<commit_message>
Created script for convert csv file into xslx
</commit_message>
<xml_diff>
--- a/utils/data/intervalliConfidenza/Test3/CI_Test3 1500ms 5sec.xlsx
+++ b/utils/data/intervalliConfidenza/Test3/CI_Test3 1500ms 5sec.xlsx
@@ -427,34 +427,34 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>120</v>
       </c>
       <c r="E2">
-        <v>72.5</v>
+        <v>68.33333333333333</v>
       </c>
       <c r="F2">
-        <v>22.541946</v>
+        <v>23.870164</v>
       </c>
       <c r="G2">
-        <v>5.427437</v>
+        <v>0.44719</v>
       </c>
       <c r="H2">
-        <v>0.5818823239742437</v>
+        <v>0.04938387414541062</v>
       </c>
       <c r="I2">
-        <v>1.140489354989518</v>
+        <v>0.09679239332500482</v>
       </c>
       <c r="J2">
-        <v>23.68243535498952</v>
+        <v>23.966956393325</v>
       </c>
       <c r="K2">
-        <v>21.40145664501048</v>
+        <v>23.773371606675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>